<commit_message>
Update files from solar experiments
</commit_message>
<xml_diff>
--- a/Code/Python/Video experiments/PWM_SPEED_RELATION.xlsx
+++ b/Code/Python/Video experiments/PWM_SPEED_RELATION.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Solar" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t xml:space="preserve">Int every 1.25 sec:</t>
   </si>
@@ -89,6 +90,21 @@
   </si>
   <si>
     <t xml:space="preserve">PWM: 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance: 75cm max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist single charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVG:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance single charge</t>
   </si>
 </sst>
 </file>
@@ -192,22 +208,22 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.20408163265306"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,4 +1167,321 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">A4/B3</f>
+        <v>23.1666666666667</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">A5/B3</f>
+        <v>23.1666666666667</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>55.7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>70.9</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">A6/B3</f>
+        <v>23.6333333333333</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>27.6</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>54.3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">A7/B3</f>
+        <v>23.3333333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">A8/B3</f>
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <f aca="false">AVERAGE(B4:B8)</f>
+        <v>23.32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>73.6</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">A13/B12</f>
+        <v>21.0285714285714</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">A14/B12</f>
+        <v>20.5142857142857</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>48.9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>72.4</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">A15/B12</f>
+        <v>20.6857142857143</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>72.8</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">A16/B12</f>
+        <v>20.8</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>50.6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>72.6</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <f aca="false">A17/B12</f>
+        <v>20.7428571428571</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <f aca="false">AVERAGE(B13:B17)</f>
+        <v>20.7542857142857</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>73.2</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <f aca="false">A22/B21</f>
+        <v>16.2666666666667</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>45.2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>69.4</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <f aca="false">A23/B21</f>
+        <v>15.4222222222222</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>73.4</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">A24/B21</f>
+        <v>16.3111111111111</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <f aca="false">A25/B21</f>
+        <v>15.6666666666667</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>74.1</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <f aca="false">A26/B21</f>
+        <v>16.4666666666667</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">AVERAGE(B22:B26)</f>
+        <v>16.0266666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standaard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Pagina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>